<commit_message>
documentacion casos de uso de prueba
</commit_message>
<xml_diff>
--- a/Documentos/cosos_de_uso_de_prueba_estadisticas..xlsx
+++ b/Documentos/cosos_de_uso_de_prueba_estadisticas..xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monit\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monit\Desktop\ProyectoIngSoftwareII-master\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21600" windowHeight="9870"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>caso de uso de prueba</t>
   </si>
@@ -139,6 +139,33 @@
   <si>
     <t>sprint 4</t>
   </si>
+  <si>
+    <t>8.11 Caso de uso de prueba Dashboard general de reportes por gerencial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.10 Caso de uso de prueba  Dashboard general de reportes por vender </t>
+  </si>
+  <si>
+    <t>8.9 Caso de uso de prueba Dashboard general de reportes por supervisar</t>
+  </si>
+  <si>
+    <t>se presentan errores con javascript ver la imagen anexa en el casod e uso</t>
+  </si>
+  <si>
+    <t>se valido de la tara a asignar no esta realizando la edicion</t>
+  </si>
+  <si>
+    <t>8.12 anexo a log in</t>
+  </si>
+  <si>
+    <t>error de la consulta a usuarios en la abse de datos</t>
+  </si>
+  <si>
+    <t>sprint 5</t>
+  </si>
+  <si>
+    <t>sprint</t>
+  </si>
 </sst>
 </file>
 
@@ -201,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -221,12 +248,48 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -589,11 +652,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="435585328"/>
-        <c:axId val="435585720"/>
+        <c:axId val="253153520"/>
+        <c:axId val="253153912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="435585328"/>
+        <c:axId val="253153520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +699,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435585720"/>
+        <c:crossAx val="253153912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -644,7 +707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="435585720"/>
+        <c:axId val="253153912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +758,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435585328"/>
+        <c:crossAx val="253153520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -937,7 +1000,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$30:$A$37</c:f>
+              <c:f>Hoja1!$A$50:$A$57</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1027,7 +1090,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$30:$A$37</c:f>
+              <c:f>Hoja1!$A$50:$A$57</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1117,7 +1180,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$30:$A$37</c:f>
+              <c:f>Hoja1!$A$50:$A$57</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1190,11 +1253,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="440471648"/>
-        <c:axId val="440473216"/>
+        <c:axId val="253152344"/>
+        <c:axId val="253156656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="440471648"/>
+        <c:axId val="253152344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1300,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440473216"/>
+        <c:crossAx val="253156656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1245,7 +1308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440473216"/>
+        <c:axId val="253156656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1359,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440471648"/>
+        <c:crossAx val="253152344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1471,7 +1534,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$A$39</c:f>
+              <c:f>Hoja1!$A$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1531,7 +1594,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$A$38</c:f>
+              <c:f>Hoja1!$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1569,6 +1632,49 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$29:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1579,11 +1685,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="439571160"/>
-        <c:axId val="439568416"/>
+        <c:axId val="253155088"/>
+        <c:axId val="253155480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="439571160"/>
+        <c:axId val="253155088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1732,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439568416"/>
+        <c:crossAx val="253155480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1634,7 +1740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="439568416"/>
+        <c:axId val="253155480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,7 +1791,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439571160"/>
+        <c:crossAx val="253155088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1699,6 +1805,935 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>casos de uso prueba</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> intentos </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$25:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.9 Caso de uso de prueba Dashboard general de reportes por supervisar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.10 Caso de uso de prueba  Dashboard general de reportes por vender </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.11 Caso de uso de prueba Dashboard general de reportes por gerencial</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.12 anexo a log in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$25:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exitoso</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$25:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.9 Caso de uso de prueba Dashboard general de reportes por supervisar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.10 Caso de uso de prueba  Dashboard general de reportes por vender </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.11 Caso de uso de prueba Dashboard general de reportes por gerencial</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.12 anexo a log in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fallido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$25:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.9 Caso de uso de prueba Dashboard general de reportes por supervisar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.10 Caso de uso de prueba  Dashboard general de reportes por vender </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.11 Caso de uso de prueba Dashboard general de reportes por gerencial</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.12 anexo a log in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$25:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="408734600"/>
+        <c:axId val="254717128"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="408734600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254717128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="254717128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="408734600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Estados del Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO" baseline="0"/>
+              <a:t> 3,4 y 5</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sprint 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$33:$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v> intentos </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>exitoso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fallido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$34:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sprint 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$33:$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v> intentos </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>exitoso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fallido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$35:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$33:$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v> intentos </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>exitoso</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fallido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$36:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="255256520"/>
+        <c:axId val="255256912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="255256520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="255256912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="255256912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="255256520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1886,6 +2921,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3363,6 +4478,1016 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3461,14 +5586,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3482,6 +5607,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3753,10 +5938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4086,54 +6271,220 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f>SUM(B25:B28)</f>
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:D29" si="1">SUM(C25:C28)</f>
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="10">
+        <f>SUM(B27:B33)</f>
+        <v>12</v>
+      </c>
+      <c r="C34" s="10">
+        <f t="shared" ref="C34:D34" si="2">SUM(C27:C33)</f>
+        <v>8</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="10">
+        <f>SUM(B27:B34)</f>
+        <v>24</v>
+      </c>
+      <c r="C35" s="10">
+        <f>SUM(C27:C34)</f>
+        <v>16</v>
+      </c>
+      <c r="D35" s="10">
+        <f>SUM(D27:D34)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="10">
+        <v>9</v>
+      </c>
+      <c r="C36" s="10">
+        <v>6</v>
+      </c>
+      <c r="D36" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>